<commit_message>
year wise sales updated with engine type
</commit_message>
<xml_diff>
--- a/data/year wise sales.xlsx
+++ b/data/year wise sales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5BB7E96-25A9-4B7B-B1E3-088D6B0981BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18D2F8AB-CC1A-4A08-9642-7DA5192FBCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>year</t>
   </si>
@@ -63,6 +63,27 @@
   </si>
   <si>
     <t>hardtop</t>
+  </si>
+  <si>
+    <t>dohcv</t>
+  </si>
+  <si>
+    <t>ohcv</t>
+  </si>
+  <si>
+    <t>ohc</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>rotor</t>
+  </si>
+  <si>
+    <t>ohcf</t>
+  </si>
+  <si>
+    <t>dohc</t>
   </si>
 </sst>
 </file>
@@ -421,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +487,29 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -504,8 +546,29 @@
       <c r="L2">
         <v>34680</v>
       </c>
+      <c r="M2">
+        <v>3462</v>
+      </c>
+      <c r="N2">
+        <v>15841</v>
+      </c>
+      <c r="O2">
+        <v>17602</v>
+      </c>
+      <c r="P2">
+        <v>14139</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1196</v>
+      </c>
+      <c r="S2">
+        <v>3263</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -542,8 +605,29 @@
       <c r="L3">
         <v>71430</v>
       </c>
+      <c r="M3">
+        <v>5025</v>
+      </c>
+      <c r="N3">
+        <v>18203</v>
+      </c>
+      <c r="O3">
+        <v>22632</v>
+      </c>
+      <c r="P3">
+        <v>11244</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1363</v>
+      </c>
+      <c r="S3">
+        <v>8184</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -580,8 +664,29 @@
       <c r="L4">
         <v>73431</v>
       </c>
+      <c r="M4">
+        <v>4582</v>
+      </c>
+      <c r="N4">
+        <v>20096</v>
+      </c>
+      <c r="O4">
+        <v>18776</v>
+      </c>
+      <c r="P4">
+        <v>2485</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1242</v>
+      </c>
+      <c r="S4">
+        <v>8312</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -617,6 +722,27 @@
       </c>
       <c r="L5">
         <v>73431</v>
+      </c>
+      <c r="M5">
+        <v>4077</v>
+      </c>
+      <c r="N5">
+        <v>21742</v>
+      </c>
+      <c r="O5">
+        <v>20091</v>
+      </c>
+      <c r="P5">
+        <v>187</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1009</v>
+      </c>
+      <c r="S5">
+        <v>8636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>